<commit_message>
Orden del sistema de ficheros
Se ordena el sistema de ficheros para su presentación
</commit_message>
<xml_diff>
--- a/ForUsers/HealthApp/Dat/RegistroMejora.xlsx
+++ b/ForUsers/HealthApp/Dat/RegistroMejora.xlsx
@@ -1,75 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Registro" sheetId="1" r:id="rId1"/>
+    <sheet name="Registro" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
-  <si>
-    <t>Fecha</t>
-  </si>
-  <si>
-    <t>dni</t>
-  </si>
-  <si>
-    <t>peso</t>
-  </si>
-  <si>
-    <t>valor</t>
-  </si>
-  <si>
-    <t>tipo</t>
-  </si>
-  <si>
-    <t>2019-05-16</t>
-  </si>
-  <si>
-    <t>2019-06-23</t>
-  </si>
-  <si>
-    <t>subir</t>
-  </si>
-  <si>
-    <t>bajar</t>
-  </si>
-  <si>
-    <t>mantener</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -84,35 +46,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -400,116 +353,173 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Fecha</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>dni</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>peso</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>valor</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>tipo</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2019-05-16</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>71308125</v>
+      </c>
+      <c r="C2" t="n">
+        <v>73.40000000000001</v>
+      </c>
+      <c r="D2" t="n">
+        <v>500</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>subir</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2019-05-16</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1234</v>
+      </c>
+      <c r="C3" t="n">
+        <v>69</v>
+      </c>
+      <c r="D3" t="n">
+        <v>500</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>subir</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2019-06-23</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>79</v>
+      </c>
+      <c r="D4" t="n">
+        <v>450</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>bajar</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2019-06-23</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>7</v>
+      </c>
+      <c r="C5" t="n">
+        <v>65</v>
+      </c>
+      <c r="D5" t="n">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>bajar</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2019-05-16</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>71308125</v>
-      </c>
-      <c r="C2">
-        <v>73.40000000000001</v>
-      </c>
-      <c r="D2">
+      <c r="C6" t="n">
+        <v>79</v>
+      </c>
+      <c r="D6" t="n">
         <v>500</v>
       </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>1234</v>
-      </c>
-      <c r="C3">
-        <v>69</v>
-      </c>
-      <c r="D3">
-        <v>500</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>79</v>
-      </c>
-      <c r="D4">
-        <v>450</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>65</v>
-      </c>
-      <c r="D5">
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>mantener</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2019-07-01</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>71308122</v>
+      </c>
+      <c r="C7" t="n">
+        <v>53</v>
+      </c>
+      <c r="D7" t="n">
         <v>0</v>
       </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>79</v>
-      </c>
-      <c r="D6">
-        <v>500</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>mantener</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>